<commit_message>
3. feladat javítókulcs kész
</commit_message>
<xml_diff>
--- a/python/3. Feladat/Javítókulcs 3. feladat.xlsx
+++ b/python/3. Feladat/Javítókulcs 3. feladat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\IKT\Alapvizsga-feladatok\python\3. Feladat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\JEDLIK\IKT\Alapvizsga-feladatok\python\3. Feladat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6647F6-E25E-467B-BF27-22DE928C7E6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EC4F6C-401A-4103-8EDA-12F894985F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adatok" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,24 @@
     <definedName name="TanulókNevei">Adatok!$A$4:$A$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
   <si>
     <t>Jelen volt</t>
   </si>
@@ -234,58 +247,61 @@
     </r>
   </si>
   <si>
-    <t>Legalább egy sort beolvasott és eltárolt az állományból.</t>
-  </si>
-  <si>
-    <t>Beolvasta és eltárolta az állomány összes sorát.</t>
-  </si>
-  <si>
-    <t>Az állományban lévő adatok alapján meghatározta az étlepon szereplő tételek számát.</t>
-  </si>
-  <si>
-    <t>Meghatározta az étlapon lévő levesek számát.</t>
-  </si>
-  <si>
-    <t>Megkereste a legolcsóbb főételt.</t>
-  </si>
-  <si>
-    <t>A legolcsóbb főétel nevét, árát és rendelt mennyiségét a képernyőre írta.</t>
-  </si>
-  <si>
-    <t>Az összes árbevételt meghatározására összegzást készített.</t>
-  </si>
-  <si>
-    <t>A szorzatösszeget jól határozta meg.</t>
-  </si>
-  <si>
-    <t>Legalább egy fajtára meghatározta a rendelések összegét.</t>
-  </si>
-  <si>
-    <t>Az összes fajtára meghatározta a rendelések összegét.</t>
-  </si>
-  <si>
-    <t>Az étel fajtákat a forrásállományból gyűjtötte ki.</t>
-  </si>
-  <si>
-    <t>Az étel nevét bekérte és eltárolta.</t>
-  </si>
-  <si>
-    <t>Szöveges állományt hozott létre menynek neve helyes.</t>
-  </si>
-  <si>
-    <t>Az állományban legalább egy étel neve szerepel helyesen.</t>
-  </si>
-  <si>
-    <t>Az állományban az összes étel neve szerepel helyesen.</t>
-  </si>
-  <si>
     <t>Teletál dolgozat</t>
   </si>
   <si>
-    <t>Tiszta kód, ha megoldott legalább 4 feladatot</t>
-  </si>
-  <si>
-    <t>A forráskódot elmentette kvalifikacio néven, a programkód szintaktikailag hibátlan, lefordítható.</t>
+    <t>Adatszerkezetet hoz létre a Monaco2023.csv adatainak eltárolására.</t>
+  </si>
+  <si>
+    <t>Az osztályban tagfüggvényt hoz létre.</t>
+  </si>
+  <si>
+    <t>Meghatározza a Q1-ben legjobb eredményt elért versenyzőt.</t>
+  </si>
+  <si>
+    <t>A minta szerint kiírta a képernyőre a Q1-ben legjobb eredményt elért versenyző adatait.</t>
+  </si>
+  <si>
+    <t>Kilistázza a képernyőre a Q2-be jutott versenyzőket, valamint az ott elért köridejüket.</t>
+  </si>
+  <si>
+    <t>Létrehozza a hatarfeletti.txt nevű állományt.</t>
+  </si>
+  <si>
+    <t>Létrehozza statisztikához szükséges objektumot.</t>
+  </si>
+  <si>
+    <t>Létrehozza a statisztikát a feladatnak megfelelően.</t>
+  </si>
+  <si>
+    <t>Kilistázza a feltételnek megfelelő konstruktőrök nevét és körideik számát.</t>
+  </si>
+  <si>
+    <t>Bekér egy köridőt.</t>
+  </si>
+  <si>
+    <t>Eltárolja a bekért köridőt.</t>
+  </si>
+  <si>
+    <t>Létrehoz egy programot kvalifikacio.py néven.</t>
+  </si>
+  <si>
+    <t>A program hibaüzenet nélkül lefut.</t>
+  </si>
+  <si>
+    <t>Meghatározza a köridők számát.</t>
+  </si>
+  <si>
+    <t>A mintának megfelelően kiírja a képernyőre a köridők számát.</t>
+  </si>
+  <si>
+    <t>A tagfüggvény a köridőt három tizedesjegy pontossággal másodpercre váltva adja vissza.</t>
+  </si>
+  <si>
+    <t>Feltételt állít konstruktőrök köridejeinket számának.</t>
+  </si>
+  <si>
+    <t>A Monaco2023.csv legalább egy sorát beolvassa.</t>
   </si>
 </sst>
 </file>
@@ -300,7 +316,7 @@
     <numFmt numFmtId="168" formatCode="0.0&quot; pt&quot;"/>
     <numFmt numFmtId="169" formatCode="General&quot; pt&quot;"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -457,20 +473,13 @@
       <charset val="238"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,8 +510,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -792,51 +807,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
@@ -848,12 +818,46 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -864,7 +868,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1130,21 +1134,9 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1200,6 +1192,15 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2831,7 +2832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E3E5BA8-BEA5-4C67-A36D-3CE806BD7A0E}" type="CELLRANGE">
+                    <a:fld id="{20A129B2-E5AE-46B3-A4EB-44BA35172F55}" type="CELLRANGE">
                       <a:rPr lang="hu-HU"/>
                       <a:pPr/>
                       <a:t>[CELLATARTOMÁNY]</a:t>
@@ -2841,7 +2842,7 @@
                       <a:t>
 </a:t>
                     </a:r>
-                    <a:fld id="{BFCCE926-75E8-44A5-A918-5082380F0A50}" type="VALUE">
+                    <a:fld id="{E3F07AEB-B427-4ADC-BFE5-182C9B41F4F4}" type="VALUE">
                       <a:rPr lang="hu-HU" baseline="0"/>
                       <a:pPr/>
                       <a:t>[ÉRTÉK]</a:t>
@@ -2877,7 +2878,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FD974B5-DB29-471F-A39A-C3385624B67D}" type="CELLRANGE">
+                    <a:fld id="{00D783C9-29AE-4FBA-B8FE-DA793FCF5C51}" type="CELLRANGE">
                       <a:rPr lang="hu-HU"/>
                       <a:pPr/>
                       <a:t>[CELLATARTOMÁNY]</a:t>
@@ -2887,7 +2888,7 @@
                       <a:t>
 </a:t>
                     </a:r>
-                    <a:fld id="{F4495B4A-0D22-4D87-A0EB-FF190FBE7449}" type="VALUE">
+                    <a:fld id="{CC3C2306-487D-494A-A67C-67E23C827852}" type="VALUE">
                       <a:rPr lang="hu-HU" baseline="0"/>
                       <a:pPr/>
                       <a:t>[ÉRTÉK]</a:t>
@@ -2923,7 +2924,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73716BBB-A2AE-4539-9FC2-5E5D82341C3E}" type="CELLRANGE">
+                    <a:fld id="{516BC9CA-2CD1-4860-8048-227E4E7590BF}" type="CELLRANGE">
                       <a:rPr lang="hu-HU"/>
                       <a:pPr/>
                       <a:t>[CELLATARTOMÁNY]</a:t>
@@ -2933,7 +2934,7 @@
                       <a:t>
 </a:t>
                     </a:r>
-                    <a:fld id="{C3FC8A6E-0473-4EED-8779-F36B57FD6482}" type="VALUE">
+                    <a:fld id="{BD0AA6C3-617F-40EA-B78F-F414AB135084}" type="VALUE">
                       <a:rPr lang="hu-HU" baseline="0"/>
                       <a:pPr/>
                       <a:t>[ÉRTÉK]</a:t>
@@ -3037,16 +3038,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0.15384615384615385</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15384615384615385</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15384615384615385</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4061,9 +4062,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4101,9 +4102,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4136,26 +4137,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4188,26 +4172,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4390,7 +4357,7 @@
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4436,251 +4403,191 @@
     <col min="46" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="28" customFormat="1" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="98" t="s">
+    <row r="1" spans="1:45" s="28" customFormat="1" ht="134.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="96" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="94" t="s">
         <v>27</v>
       </c>
       <c r="E1" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="84" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="85" t="s">
+      <c r="F1" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="100" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="100" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="100" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="100" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="100" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" s="100" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" s="100" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="100" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" s="100" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="88" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="86" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="85" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="86" t="s">
-        <v>64</v>
-      </c>
-      <c r="N1" s="86" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="85" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" s="84" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" s="86" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" s="84" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" s="86" t="s">
-        <v>67</v>
-      </c>
-      <c r="U1" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="V1" s="84" t="s">
-        <v>44</v>
-      </c>
-      <c r="W1" s="86" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" s="85" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y1" s="84" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z1" s="86" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA1" s="86" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB1" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC1" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD1" s="86" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE1" s="86" t="s">
+      <c r="W1" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="AF1" s="86" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG1" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH1" s="84" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI1" s="86" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ1" s="86" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK1" s="86" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL1" s="85" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM1" s="87" t="s">
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
+      <c r="AC1" s="100"/>
+      <c r="AD1" s="100"/>
+      <c r="AE1" s="100"/>
+      <c r="AF1" s="100"/>
+      <c r="AG1" s="100"/>
+      <c r="AH1" s="100"/>
+      <c r="AI1" s="100"/>
+      <c r="AJ1" s="100"/>
+      <c r="AK1" s="100"/>
+      <c r="AL1" s="101"/>
+      <c r="AM1" s="84" t="s">
         <v>21</v>
       </c>
       <c r="AN1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="AO1" s="92" t="s">
+      <c r="AO1" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="AP1" s="93"/>
-      <c r="AQ1" s="96">
+      <c r="AP1" s="89"/>
+      <c r="AQ1" s="92">
         <f>IF(COUNT(4:35)&gt;0,AVERAGE(AQ4:AQ35),"-")</f>
         <v>1</v>
       </c>
-      <c r="AR1" s="89"/>
+      <c r="AR1" s="85"/>
       <c r="AS1" s="27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="101"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
+    <row r="2" spans="1:45" s="33" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="97"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
       <c r="E2" s="29"/>
       <c r="F2" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2" s="83">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I2" s="83">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2" s="83">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K2" s="83">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L2" s="83">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M2" s="83">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N2" s="83">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="O2" s="83">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P2" s="83">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="Q2" s="83">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="R2" s="83">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="S2" s="83">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="T2" s="83">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="U2" s="83">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="V2" s="83">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="W2" s="83">
-        <v>5</v>
-      </c>
-      <c r="X2" s="83">
-        <v>5</v>
-      </c>
-      <c r="Y2" s="83">
-        <v>6</v>
-      </c>
-      <c r="Z2" s="83">
-        <v>6</v>
-      </c>
-      <c r="AA2" s="83">
-        <v>6</v>
-      </c>
-      <c r="AB2" s="83">
-        <v>6</v>
-      </c>
-      <c r="AC2" s="83">
-        <v>7</v>
-      </c>
-      <c r="AD2" s="83">
-        <v>7</v>
-      </c>
-      <c r="AE2" s="83">
-        <v>7</v>
-      </c>
-      <c r="AF2" s="83">
-        <v>7</v>
-      </c>
-      <c r="AG2" s="83">
-        <v>7</v>
-      </c>
-      <c r="AH2" s="83">
-        <v>8</v>
-      </c>
-      <c r="AI2" s="83">
-        <v>8</v>
-      </c>
-      <c r="AJ2" s="83">
-        <v>8</v>
-      </c>
-      <c r="AK2" s="83">
-        <v>8</v>
-      </c>
-      <c r="AL2" s="83">
-        <v>8</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+      <c r="AA2" s="83"/>
+      <c r="AB2" s="83"/>
+      <c r="AC2" s="83"/>
+      <c r="AD2" s="83"/>
+      <c r="AE2" s="83"/>
+      <c r="AF2" s="83"/>
+      <c r="AG2" s="83"/>
+      <c r="AH2" s="83"/>
+      <c r="AI2" s="83"/>
+      <c r="AJ2" s="83"/>
+      <c r="AK2" s="83"/>
+      <c r="AL2" s="83"/>
       <c r="AM2" s="30"/>
       <c r="AN2" s="31"/>
-      <c r="AO2" s="94"/>
-      <c r="AP2" s="95"/>
-      <c r="AQ2" s="97"/>
-      <c r="AR2" s="90"/>
+      <c r="AO2" s="90"/>
+      <c r="AP2" s="91"/>
+      <c r="AQ2" s="93"/>
+      <c r="AR2" s="86"/>
       <c r="AS2" s="32">
         <v>0.02</v>
       </c>
@@ -4696,7 +4603,7 @@
       <c r="D3" s="55"/>
       <c r="E3" s="36"/>
       <c r="F3" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="37">
         <v>1</v>
@@ -4705,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="37">
         <v>1</v>
@@ -4714,7 +4621,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="37">
         <v>1</v>
@@ -4726,7 +4633,7 @@
         <v>1</v>
       </c>
       <c r="P3" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="37">
         <v>1</v>
@@ -4735,65 +4642,35 @@
         <v>1</v>
       </c>
       <c r="S3" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U3" s="37">
         <v>1</v>
       </c>
       <c r="V3" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" s="37">
-        <v>2</v>
-      </c>
-      <c r="X3" s="37">
         <v>1</v>
       </c>
-      <c r="Y3" s="37">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="37">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="37">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="37">
-        <v>1</v>
-      </c>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37"/>
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
       <c r="AM3" s="36">
         <v>0</v>
       </c>
@@ -4802,7 +4679,7 @@
       </c>
       <c r="AO3" s="38">
         <f>SUM($F3:AL3)+$E$3+$AM$3+$AN$3</f>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="AP3" s="39">
         <f t="shared" ref="AP3" si="0">AO3/$AO$3</f>
@@ -4855,27 +4732,19 @@
       <c r="AF4" s="58"/>
       <c r="AG4" s="58"/>
       <c r="AH4" s="58"/>
-      <c r="AI4" s="58">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="58">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="58">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="58">
-        <v>1</v>
-      </c>
+      <c r="AI4" s="58"/>
+      <c r="AJ4" s="58"/>
+      <c r="AK4" s="58"/>
+      <c r="AL4" s="58"/>
       <c r="AM4" s="57"/>
       <c r="AN4" s="57"/>
       <c r="AO4" s="59">
         <f>IF($C4="ü",SUM($F4:AL4)+$E4+$AM4+$AN4,"")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AP4" s="60">
         <f>IF($C4="ü",AO4/AO$3,"")</f>
-        <v>0.15384615384615385</v>
+        <v>0</v>
       </c>
       <c r="AQ4" s="56">
         <f>IF($C4="ü",VLOOKUP(AP4,Jegyek!$A$2:$D$7,3),"-")</f>
@@ -4924,18 +4793,10 @@
       <c r="AF5" s="77"/>
       <c r="AG5" s="77"/>
       <c r="AH5" s="77"/>
-      <c r="AI5" s="77">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="77">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="77">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="77">
-        <v>0</v>
-      </c>
+      <c r="AI5" s="77"/>
+      <c r="AJ5" s="77"/>
+      <c r="AK5" s="77"/>
+      <c r="AL5" s="77"/>
       <c r="AM5" s="76"/>
       <c r="AN5" s="76"/>
       <c r="AO5" s="59">
@@ -4990,27 +4851,19 @@
       <c r="AF6" s="65"/>
       <c r="AG6" s="65"/>
       <c r="AH6" s="65"/>
-      <c r="AI6" s="65">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="65">
-        <v>1</v>
-      </c>
-      <c r="AK6" s="65">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="65">
-        <v>1</v>
-      </c>
+      <c r="AI6" s="65"/>
+      <c r="AJ6" s="65"/>
+      <c r="AK6" s="65"/>
+      <c r="AL6" s="65"/>
       <c r="AM6" s="64"/>
       <c r="AN6" s="64"/>
       <c r="AO6" s="59">
         <f>IF($C6="ü",SUM($F6:AL6)+$E6+$AM6+$AN6,"")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AP6" s="60">
         <f t="shared" ref="AP6" si="2">IF($C6="ü",AO6/AO$3,"")</f>
-        <v>0.15384615384615385</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="56">
         <f>IF($C6="ü",VLOOKUP(AP6,Jegyek!$A$2:$D$7,3),"-")</f>
@@ -5059,27 +4912,19 @@
       <c r="AF7" s="65"/>
       <c r="AG7" s="65"/>
       <c r="AH7" s="65"/>
-      <c r="AI7" s="65">
-        <v>1</v>
-      </c>
-      <c r="AJ7" s="65">
-        <v>1</v>
-      </c>
-      <c r="AK7" s="65">
-        <v>1</v>
-      </c>
-      <c r="AL7" s="65">
-        <v>1</v>
-      </c>
+      <c r="AI7" s="65"/>
+      <c r="AJ7" s="65"/>
+      <c r="AK7" s="65"/>
+      <c r="AL7" s="65"/>
       <c r="AM7" s="64"/>
       <c r="AN7" s="64"/>
       <c r="AO7" s="59">
         <f>IF($C7="ü",SUM($F7:AL7)+$E7+$AM7+$AN7,"")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AP7" s="60">
         <f t="shared" ref="AP7:AP35" si="3">IF($C7="ü",AO7/AO$3,"")</f>
-        <v>0.15384615384615385</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="56">
         <f>IF($C7="ü",VLOOKUP(AP7,Jegyek!$A$2:$D$7,3),"-")</f>
@@ -6809,11 +6654,11 @@
       <c r="AN36" s="45"/>
       <c r="AO36" s="43">
         <f>IF(COUNT(AO4:AO35)&gt;0,AVERAGE(AO4:AO35),"-")</f>
-        <v>0.70588235294117652</v>
+        <v>0</v>
       </c>
       <c r="AP36" s="44">
         <f>IF(COUNT(AP4:AP35)&gt;0,AVERAGE(AP4:AP35),"-")</f>
-        <v>2.7149321266968326E-2</v>
+        <v>0</v>
       </c>
       <c r="AQ36" s="45">
         <f>IF(COUNT(AQ4:AQ35)&gt;0,AVERAGE(AQ4:AQ35),"-")</f>
@@ -6823,11 +6668,11 @@
       <c r="AS36" s="48"/>
     </row>
     <row r="37" spans="1:45" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="91" t="s">
+      <c r="A37" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="87"/>
       <c r="E37" s="49" t="str">
         <f>IF(COUNT(E$4:E35)&gt;0,AVERAGE(E$4:E35),"-")</f>
         <v>-</v>
@@ -6945,21 +6790,21 @@
         <f>IF(COUNT(AH$4:AH35)&gt;0,AVERAGE(AH$4:AH35),"-")</f>
         <v>-</v>
       </c>
-      <c r="AI37" s="49">
+      <c r="AI37" s="49" t="str">
         <f>IF(COUNT(AI$4:AI35)&gt;0,AVERAGE(AI$4:AI35),"-")</f>
-        <v>0.75</v>
-      </c>
-      <c r="AJ37" s="49">
+        <v>-</v>
+      </c>
+      <c r="AJ37" s="49" t="str">
         <f>IF(COUNT(AJ$4:AJ35)&gt;0,AVERAGE(AJ$4:AJ35),"-")</f>
-        <v>0.75</v>
-      </c>
-      <c r="AK37" s="49">
+        <v>-</v>
+      </c>
+      <c r="AK37" s="49" t="str">
         <f>IF(COUNT(AK$4:AK35)&gt;0,AVERAGE(AK$4:AK35),"-")</f>
-        <v>0.75</v>
-      </c>
-      <c r="AL37" s="49">
+        <v>-</v>
+      </c>
+      <c r="AL37" s="49" t="str">
         <f>IF(COUNT(AL$4:AL35)&gt;0,AVERAGE(AL$4:AL35),"-")</f>
-        <v>0.75</v>
+        <v>-</v>
       </c>
       <c r="AM37" s="49" t="str">
         <f>IF(COUNT(AM$4:AM35)&gt;0,AVERAGE(AM$4:AM35),"-")</f>
@@ -6971,11 +6816,11 @@
       </c>
     </row>
     <row r="38" spans="1:45" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="91" t="s">
+      <c r="A38" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="91"/>
-      <c r="C38" s="91"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="87"/>
       <c r="E38" s="49" t="str">
         <f>IF(COUNT(E$4:E35)&gt;0,_xlfn.STDEV.P(E$4:E35),"-")</f>
         <v>-</v>
@@ -7093,21 +6938,21 @@
         <f>IF(COUNT(AH$4:AH35)&gt;0,_xlfn.STDEV.P(AH$4:AH35),"-")</f>
         <v>-</v>
       </c>
-      <c r="AI38" s="49">
+      <c r="AI38" s="49" t="str">
         <f>IF(COUNT(AI$4:AI35)&gt;0,_xlfn.STDEV.P(AI$4:AI35),"-")</f>
-        <v>0.4330127018922193</v>
-      </c>
-      <c r="AJ38" s="49">
+        <v>-</v>
+      </c>
+      <c r="AJ38" s="49" t="str">
         <f>IF(COUNT(AJ$4:AJ35)&gt;0,_xlfn.STDEV.P(AJ$4:AJ35),"-")</f>
-        <v>0.4330127018922193</v>
-      </c>
-      <c r="AK38" s="49">
+        <v>-</v>
+      </c>
+      <c r="AK38" s="49" t="str">
         <f>IF(COUNT(AK$4:AK35)&gt;0,_xlfn.STDEV.P(AK$4:AK35),"-")</f>
-        <v>0.4330127018922193</v>
-      </c>
-      <c r="AL38" s="49">
+        <v>-</v>
+      </c>
+      <c r="AL38" s="49" t="str">
         <f>IF(COUNT(AL$4:AL35)&gt;0,_xlfn.STDEV.P(AL$4:AL35),"-")</f>
-        <v>0.4330127018922193</v>
+        <v>-</v>
       </c>
       <c r="AM38" s="49" t="str">
         <f>IF(COUNT(AM$4:AM35)&gt;0,_xlfn.STDEV.P(AM$4:AM35),"-")</f>
@@ -7119,11 +6964,11 @@
       </c>
     </row>
     <row r="39" spans="1:45" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="91" t="s">
+      <c r="A39" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="91"/>
-      <c r="C39" s="91"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="87"/>
       <c r="E39" s="50" t="str">
         <f>IF(COUNT(E$4:E35)&gt;0,COUNTIF(E$4:E35,"="&amp;E$3),"-")</f>
         <v>-</v>
@@ -7241,21 +7086,21 @@
         <f>IF(COUNT(AH$4:AH35)&gt;0,COUNTIF(AH$4:AH35,"="&amp;#REF!),"-")</f>
         <v>-</v>
       </c>
-      <c r="AI39" s="50">
+      <c r="AI39" s="50" t="str">
         <f>IF(COUNT(AI$4:AI35)&gt;0,COUNTIF(AI$4:AI35,"="&amp;#REF!),"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ39" s="50">
+        <v>-</v>
+      </c>
+      <c r="AJ39" s="50" t="str">
         <f>IF(COUNT(AJ$4:AJ35)&gt;0,COUNTIF(AJ$4:AJ35,"="&amp;#REF!),"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AK39" s="50">
+        <v>-</v>
+      </c>
+      <c r="AK39" s="50" t="str">
         <f>IF(COUNT(AK$4:AK35)&gt;0,COUNTIF(AK$4:AK35,"="&amp;#REF!),"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AL39" s="50">
+        <v>-</v>
+      </c>
+      <c r="AL39" s="50" t="str">
         <f>IF(COUNT(AL$4:AL35)&gt;0,COUNTIF(AL$4:AL35,"="&amp;#REF!),"-")</f>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="AM39" s="50" t="str">
         <f>IF(COUNT(AM$4:AM35)&gt;0,COUNTIF(AM$4:AM35,"="&amp;AM$3),"-")</f>
@@ -7267,11 +7112,11 @@
       </c>
     </row>
     <row r="40" spans="1:45" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="91" t="s">
+      <c r="A40" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="91"/>
-      <c r="C40" s="91"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="87"/>
       <c r="E40" s="51" t="str">
         <f>IF(COUNT(E$4:E35)&gt;0,COUNTIF(E$4:E35,"&lt;"&amp;E$3),"-")</f>
         <v>-</v>
@@ -7389,21 +7234,21 @@
         <f>IF(COUNT(AH$4:AH35)&gt;0,COUNTIF(AH$4:AH35,"&lt;"&amp;#REF!),"-")</f>
         <v>-</v>
       </c>
-      <c r="AI40" s="51">
+      <c r="AI40" s="51" t="str">
         <f>IF(COUNT(AI$4:AI35)&gt;0,COUNTIF(AI$4:AI35,"&lt;"&amp;#REF!),"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ40" s="51">
+        <v>-</v>
+      </c>
+      <c r="AJ40" s="51" t="str">
         <f>IF(COUNT(AJ$4:AJ35)&gt;0,COUNTIF(AJ$4:AJ35,"&lt;"&amp;#REF!),"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AK40" s="51">
+        <v>-</v>
+      </c>
+      <c r="AK40" s="51" t="str">
         <f>IF(COUNT(AK$4:AK35)&gt;0,COUNTIF(AK$4:AK35,"&lt;"&amp;#REF!),"-")</f>
-        <v>0</v>
-      </c>
-      <c r="AL40" s="51">
+        <v>-</v>
+      </c>
+      <c r="AL40" s="51" t="str">
         <f>IF(COUNT(AL$4:AL35)&gt;0,COUNTIF(AL$4:AL35,"&lt;"&amp;#REF!),"-")</f>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="AM40" s="51" t="str">
         <f>IF(COUNT(AM$4:AM35)&gt;0,COUNTIF(AM$4:AM35,"&lt;"&amp;AM$3),"-")</f>
@@ -7419,29 +7264,29 @@
       <c r="B41" s="53"/>
     </row>
     <row r="42" spans="1:45" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="91" t="s">
+      <c r="A42" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="91"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="87"/>
       <c r="E42" s="54">
         <f>IFERROR(INDEX($A$4:$AP35,MATCH(MAX($AP$4:$AP35),$AP$4:$AP35,0),1),"-")</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:45" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="91" t="s">
+      <c r="A43" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="91"/>
-      <c r="C43" s="91"/>
+      <c r="B43" s="87"/>
+      <c r="C43" s="87"/>
       <c r="E43" s="54">
         <f>IFERROR(INDEX($A$4:$AP35,MATCH(MIN($AP$4:$AP35),$AP$4:$AP35,0),1),"-")</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:U20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:U20">
     <sortCondition ref="A4:A20"/>
   </sortState>
   <mergeCells count="13">
@@ -7478,7 +7323,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37:H37 AH37:AL37 J37:AB37">
+  <conditionalFormatting sqref="G37:H37 J37:AB37 AH37:AL37">
     <cfRule type="cellIs" dxfId="3" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
@@ -7769,7 +7614,7 @@
       </c>
       <c r="B2" s="14">
         <f>ROUNDUP(Adatok!$AO$3*Jegyek!A2,1)</f>
-        <v>-260</v>
+        <v>-180</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
@@ -7814,7 +7659,7 @@
       </c>
       <c r="B4" s="14">
         <f>ROUNDUP(Adatok!$AO$3*Jegyek!A4,1)</f>
-        <v>10.4</v>
+        <v>7.2</v>
       </c>
       <c r="C4" s="9">
         <v>2</v>
@@ -7830,7 +7675,7 @@
       </c>
       <c r="B5" s="14">
         <f>ROUNDUP(Adatok!$AO$3*Jegyek!A5,1)</f>
-        <v>14.3</v>
+        <v>9.9</v>
       </c>
       <c r="C5" s="9">
         <v>3</v>
@@ -7846,7 +7691,7 @@
       </c>
       <c r="B6" s="14">
         <f>ROUNDUP(Adatok!$AO$3*Jegyek!A6,1)</f>
-        <v>18.2</v>
+        <v>12.6</v>
       </c>
       <c r="C6" s="9">
         <v>4</v>
@@ -7862,7 +7707,7 @@
       </c>
       <c r="B7" s="14">
         <f>ROUNDUP(Adatok!$AO$3*Jegyek!A7,1)</f>
-        <v>22.1</v>
+        <v>15.3</v>
       </c>
       <c r="C7" s="9">
         <v>5</v>
@@ -7875,7 +7720,7 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
         <f>Adatok!AO3</f>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C10" s="11">
         <f>B10/$B$10</f>
@@ -7886,10 +7731,10 @@
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="102"/>
+      <c r="C11" s="98"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -7996,7 +7841,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C18" s="13">
         <f>IF(COUNT(Adatok!AP4:AP35)&gt;0,AVERAGE(Adatok!AP4:AP35),"-")</f>
-        <v>2.7149321266968326E-2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>